<commit_message>
find excel table in test
</commit_message>
<xml_diff>
--- a/debug_data.xlsx
+++ b/debug_data.xlsx
@@ -599,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -658,6 +658,12 @@
       <color theme="1"/>
       <name val="Vazirmatn"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Vazirmatn"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -711,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -886,6 +892,9 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -966,8 +975,14 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="2">
+  <tableStyles count="3">
     <tableStyle count="4" pivot="0" name="Sheet1-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="Sheet2-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1023,7 +1038,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F15" displayName="Table2" name="Table2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C9" displayName="Table3" name="Table3" id="2">
+  <tableColumns count="3">
+    <tableColumn name="چه محصولی فروختیم" id="1"/>
+    <tableColumn name="مبلغ" id="2"/>
+    <tableColumn name="درصد" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F15" displayName="Table2" name="Table2" id="3">
   <tableColumns count="6">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -10571,101 +10597,107 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" ht="22.5" customHeight="1">
+      <c r="A1" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="58" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="58" t="s">
+    <row r="2" ht="22.5" customHeight="1">
+      <c r="A2" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="60">
         <v>1300.0</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="61">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="58" t="s">
+    <row r="3" ht="22.5" customHeight="1">
+      <c r="A3" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="60">
         <v>38000.0</v>
       </c>
-      <c r="C3" s="60">
+      <c r="C3" s="61">
         <v>43.7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="58" t="s">
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="60">
         <v>19000.0</v>
       </c>
-      <c r="C4" s="60">
+      <c r="C4" s="61">
         <v>21.8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="58" t="s">
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="60">
         <v>19000.0</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="61">
         <v>21.8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="58" t="s">
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="60">
         <v>7000.0</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="61">
         <v>8.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="58" t="s">
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="A7" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="60">
         <v>2700.0</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="61">
         <v>3.1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="61"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="62"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="61"/>
-      <c r="B9" s="59">
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="62"/>
+      <c r="B9" s="60">
         <v>87000.0</v>
       </c>
-      <c r="C9" s="62"/>
+      <c r="C9" s="63"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -10686,136 +10718,136 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="64" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
     </row>
     <row r="4" ht="22.5" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
     </row>
     <row r="6" ht="22.5" customHeight="1">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="A9" s="64"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
     </row>
     <row r="11" ht="22.5" customHeight="1">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
     </row>
     <row r="12" ht="22.5" customHeight="1">
-      <c r="A12" s="64"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
     </row>
     <row r="13" ht="22.5" customHeight="1">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="A15" s="64"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>